<commit_message>
J'essaye les interfaces graphiques.
</commit_message>
<xml_diff>
--- a/CorrectionTP3-TP4.xlsx
+++ b/CorrectionTP3-TP4.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\IFT1004\IFT1004_E2017\TPs\TP3-TP4 E17\TP3 et TP4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015" tabRatio="709"/>
+    <workbookView xWindow="-38400" yWindow="-4060" windowWidth="38400" windowHeight="21600" tabRatio="709"/>
   </bookViews>
   <sheets>
     <sheet name="TP3" sheetId="48" r:id="rId1"/>
@@ -18,12 +13,17 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>Barême</t>
   </si>
@@ -260,13 +260,25 @@
   </si>
   <si>
     <t>Nom et prénom de chaque  coéquipier:</t>
+  </si>
+  <si>
+    <t>Anthony Gagnon</t>
+  </si>
+  <si>
+    <t>Louis Cusson</t>
+  </si>
+  <si>
+    <t>111 129 416</t>
+  </si>
+  <si>
+    <t>111 142 104</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +360,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -367,16 +384,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -384,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -414,6 +431,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,7 +524,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -555,7 +576,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -781,7 +802,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J80"/>
@@ -790,39 +811,50 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="58.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="90.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="58.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="90.83203125" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16">
+      <c r="B2" s="16" t="s">
+        <v>80</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="6" t="s">
         <v>77</v>
       </c>
@@ -837,7 +869,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15">
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
@@ -849,7 +881,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18">
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
@@ -860,12 +892,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="18">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="14" t="s">
         <v>44</v>
       </c>
@@ -874,7 +906,7 @@
       </c>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="14" t="s">
         <v>14</v>
       </c>
@@ -882,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
@@ -890,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -898,7 +930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
@@ -906,7 +938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" s="9" t="s">
         <v>10</v>
       </c>
@@ -914,7 +946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
@@ -922,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" s="14" t="s">
         <v>47</v>
       </c>
@@ -930,7 +962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="14" t="s">
         <v>46</v>
       </c>
@@ -938,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="13" t="s">
         <v>45</v>
       </c>
@@ -946,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15">
       <c r="A23" s="5" t="s">
         <v>2</v>
       </c>
@@ -959,14 +991,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="18">
       <c r="A25" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" s="14" t="s">
         <v>48</v>
       </c>
@@ -974,7 +1006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15">
       <c r="A27" s="14" t="s">
         <v>14</v>
       </c>
@@ -982,7 +1014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15">
       <c r="A28" s="9" t="s">
         <v>16</v>
       </c>
@@ -990,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15">
       <c r="A29" s="9" t="s">
         <v>17</v>
       </c>
@@ -998,7 +1030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" s="9" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15">
       <c r="A31" s="9" t="s">
         <v>18</v>
       </c>
@@ -1014,7 +1046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15">
       <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
@@ -1022,10 +1054,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15">
       <c r="A33" s="13"/>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15">
       <c r="A34" s="5" t="s">
         <v>2</v>
       </c>
@@ -1038,18 +1070,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="18">
       <c r="A36" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" s="14" t="s">
         <v>49</v>
       </c>
@@ -1057,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15">
       <c r="A38" s="9" t="s">
         <v>14</v>
       </c>
@@ -1065,7 +1097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15">
       <c r="A39" s="9" t="s">
         <v>21</v>
       </c>
@@ -1073,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15">
       <c r="A40" s="9" t="s">
         <v>22</v>
       </c>
@@ -1081,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15">
       <c r="A41" s="9" t="s">
         <v>10</v>
       </c>
@@ -1089,7 +1121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15">
       <c r="A42" s="9" t="s">
         <v>19</v>
       </c>
@@ -1097,10 +1129,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15">
       <c r="A43" s="13"/>
     </row>
-    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
@@ -1113,18 +1145,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
     </row>
-    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="18">
       <c r="A46" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15">
       <c r="A47" s="9" t="s">
         <v>24</v>
       </c>
@@ -1132,7 +1164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15">
       <c r="A48" s="9" t="s">
         <v>23</v>
       </c>
@@ -1140,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15">
       <c r="A49" s="9" t="s">
         <v>25</v>
       </c>
@@ -1148,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15">
       <c r="A50" s="9" t="s">
         <v>26</v>
       </c>
@@ -1156,7 +1188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="15">
       <c r="A51" s="9" t="s">
         <v>27</v>
       </c>
@@ -1164,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="15">
       <c r="A52" s="9" t="s">
         <v>28</v>
       </c>
@@ -1172,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="15">
       <c r="A53" s="9" t="s">
         <v>29</v>
       </c>
@@ -1180,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="15">
       <c r="A54" s="9" t="s">
         <v>30</v>
       </c>
@@ -1188,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="15">
       <c r="A55" s="14" t="s">
         <v>50</v>
       </c>
@@ -1196,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="15">
       <c r="A56" s="14" t="s">
         <v>51</v>
       </c>
@@ -1204,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="15">
       <c r="A57" s="14" t="s">
         <v>52</v>
       </c>
@@ -1212,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="15">
       <c r="A58" s="5" t="s">
         <v>2</v>
       </c>
@@ -1225,14 +1257,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="18">
       <c r="A60" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="15">
       <c r="A61" s="9" t="s">
         <v>34</v>
       </c>
@@ -1240,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="15">
       <c r="A62" s="9" t="s">
         <v>35</v>
       </c>
@@ -1248,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="15">
       <c r="A63" s="9" t="s">
         <v>36</v>
       </c>
@@ -1256,7 +1288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="15">
       <c r="A64" s="9" t="s">
         <v>37</v>
       </c>
@@ -1264,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15">
       <c r="A65" s="9" t="s">
         <v>53</v>
       </c>
@@ -1272,7 +1304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15">
       <c r="A66" s="9" t="s">
         <v>30</v>
       </c>
@@ -1280,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="15">
       <c r="A67" s="9" t="s">
         <v>38</v>
       </c>
@@ -1288,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="15">
       <c r="A68" s="9" t="s">
         <v>39</v>
       </c>
@@ -1296,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="15">
       <c r="A69" s="5" t="s">
         <v>2</v>
       </c>
@@ -1309,14 +1341,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="18">
       <c r="A71" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15">
       <c r="A72" s="9" t="s">
         <v>40</v>
       </c>
@@ -1324,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15">
       <c r="A73" s="9" t="s">
         <v>54</v>
       </c>
@@ -1332,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15">
       <c r="A74" s="9" t="s">
         <v>35</v>
       </c>
@@ -1340,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="15">
       <c r="A75" s="9" t="s">
         <v>36</v>
       </c>
@@ -1348,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="15">
       <c r="A76" s="9" t="s">
         <v>30</v>
       </c>
@@ -1356,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="15">
       <c r="A77" s="9" t="s">
         <v>41</v>
       </c>
@@ -1364,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="15">
       <c r="A78" s="9" t="s">
         <v>42</v>
       </c>
@@ -1372,10 +1404,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="15">
       <c r="A79" s="9"/>
     </row>
-    <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="15">
       <c r="A80" s="5" t="s">
         <v>2</v>
       </c>
@@ -1390,7 +1422,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="59" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="59" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1402,32 +1439,32 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="63" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="84.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="84.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16">
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="16">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="6" t="s">
         <v>77</v>
       </c>
@@ -1442,7 +1479,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15">
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1454,7 +1491,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>0</v>
@@ -1466,12 +1503,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="30">
       <c r="A13" s="11" t="s">
         <v>55</v>
       </c>
@@ -1480,7 +1517,7 @@
       </c>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="11" t="s">
         <v>56</v>
       </c>
@@ -1488,7 +1525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="11" t="s">
         <v>57</v>
       </c>
@@ -1496,7 +1533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="11" t="s">
         <v>58</v>
       </c>
@@ -1504,11 +1541,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="13"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1521,14 +1558,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="18">
       <c r="A20" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="11" t="s">
         <v>59</v>
       </c>
@@ -1536,7 +1573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="11" t="s">
         <v>60</v>
       </c>
@@ -1544,7 +1581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15">
       <c r="A23" s="11" t="s">
         <v>61</v>
       </c>
@@ -1552,7 +1589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15">
       <c r="A24" s="11" t="s">
         <v>62</v>
       </c>
@@ -1560,7 +1597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15">
       <c r="A25" s="11" t="s">
         <v>63</v>
       </c>
@@ -1568,7 +1605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" s="11" t="s">
         <v>64</v>
       </c>
@@ -1576,7 +1613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15">
       <c r="A27" s="11" t="s">
         <v>65</v>
       </c>
@@ -1584,7 +1621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15">
       <c r="A28" s="11" t="s">
         <v>67</v>
       </c>
@@ -1592,7 +1629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15">
       <c r="A29" s="11" t="s">
         <v>66</v>
       </c>
@@ -1600,7 +1637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" s="11" t="s">
         <v>68</v>
       </c>
@@ -1608,7 +1645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15">
       <c r="A31" s="11" t="s">
         <v>69</v>
       </c>
@@ -1616,7 +1653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15">
       <c r="A32" s="11" t="s">
         <v>70</v>
       </c>
@@ -1624,7 +1661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15">
       <c r="A33" s="11" t="s">
         <v>72</v>
       </c>
@@ -1632,7 +1669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15">
       <c r="A34" s="11" t="s">
         <v>71</v>
       </c>
@@ -1640,10 +1677,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15">
       <c r="A35" s="11"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15">
       <c r="A36" s="5" t="s">
         <v>2</v>
       </c>
@@ -1656,18 +1693,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" s="5"/>
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="18">
       <c r="A38" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15">
       <c r="A39" s="11" t="s">
         <v>73</v>
       </c>
@@ -1675,7 +1712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15">
       <c r="A40" s="11" t="s">
         <v>74</v>
       </c>
@@ -1683,10 +1720,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15">
       <c r="A41" s="13"/>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -1699,12 +1736,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
On est en train de valider le tout
</commit_message>
<xml_diff>
--- a/CorrectionTP3-TP4.xlsx
+++ b/CorrectionTP3-TP4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4060" windowWidth="38400" windowHeight="21600" tabRatio="709"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="709"/>
   </bookViews>
   <sheets>
     <sheet name="TP3" sheetId="48" r:id="rId1"/>
@@ -366,12 +366,18 @@
       <name val="Times"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -401,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -428,13 +434,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,8 +816,8 @@
   </sheetPr>
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -829,12 +838,12 @@
       <c r="A1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>80</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -845,12 +854,12 @@
       <c r="A3" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>82</v>
       </c>
     </row>
@@ -861,7 +870,7 @@
       <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <f>C23+C34+C44+C58+C69+C80</f>
         <v>0</v>
       </c>
@@ -873,7 +882,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <f>B23+B34+B44+B58+B69+B80</f>
         <v>80</v>
       </c>
@@ -898,7 +907,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="7">
@@ -907,7 +916,7 @@
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B14">
@@ -915,7 +924,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B15">
@@ -923,7 +932,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B16">
@@ -931,7 +940,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B17">
@@ -947,7 +956,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B19">
@@ -955,7 +964,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B20">
@@ -963,7 +972,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B21">
@@ -971,7 +980,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="18" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="6">
@@ -999,7 +1008,7 @@
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="15">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B26">
@@ -1007,7 +1016,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B27">
@@ -1015,7 +1024,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B28">
@@ -1023,7 +1032,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B29">
@@ -1039,7 +1048,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="15">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B31">
@@ -1047,7 +1056,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B32">
@@ -1082,7 +1091,7 @@
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" ht="15">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="17" t="s">
         <v>49</v>
       </c>
       <c r="B37">
@@ -1090,7 +1099,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="15">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B38">
@@ -1098,7 +1107,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="15">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B39">
@@ -1106,7 +1115,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="15">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B40">
@@ -1122,7 +1131,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="15">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B42">
@@ -1157,7 +1166,7 @@
       <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:3" ht="15">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B47">
@@ -1165,7 +1174,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="15">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B48">
@@ -1173,7 +1182,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="15">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B49">
@@ -1181,7 +1190,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B50">
@@ -1189,7 +1198,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B51">
@@ -1197,7 +1206,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B52">
@@ -1205,7 +1214,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B53">
@@ -1213,7 +1222,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B54">
@@ -1221,7 +1230,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="17" t="s">
         <v>50</v>
       </c>
       <c r="B55">
@@ -1229,7 +1238,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="15">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="17" t="s">
         <v>51</v>
       </c>
       <c r="B56">
@@ -1237,7 +1246,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="15">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B57">
@@ -1471,7 +1480,7 @@
       <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <f>C18+C36+C42</f>
         <v>0</v>
       </c>
@@ -1483,7 +1492,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <f>B18+B36+B42</f>
         <v>80</v>
       </c>

</xml_diff>